<commit_message>
Theory Integration Update 09/09/2025
Updated mapping and adding theory characteristics
</commit_message>
<xml_diff>
--- a/definitions/Final Constructs (Across Theory Mapping).xlsx
+++ b/definitions/Final Constructs (Across Theory Mapping).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uzh-my.sharepoint.com/personal/maya_braun_uzh_ch/Documents/git/theory-database/definitions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac.sharepoint.com/sites/APRICOTTeamHub/Shared Documents/Research/WP2 Extend the BCIO/Theory Integration/BCIO changes from construct mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="381" documentId="8_{A5CF48E9-013B-48E3-B2A5-3B394B69ECB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A90F4752-CCD5-4464-B16D-8AE94463FE31}"/>
+  <xr:revisionPtr revIDLastSave="385" documentId="8_{A5CF48E9-013B-48E3-B2A5-3B394B69ECB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16889E83-6F9C-4B47-83B0-8F247BED4A62}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19804" uniqueCount="4839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19804" uniqueCount="4840">
   <si>
     <t>Theory No.</t>
   </si>
@@ -14301,9 +14301,6 @@
     <t>The absence of intentional motivation or goal-directed behavior, often characterized by a lack of perceived control, purpose, or relevance in one's actions.</t>
   </si>
   <si>
-    <t>BCIO:050961</t>
-  </si>
-  <si>
     <t>Social contexts</t>
   </si>
   <si>
@@ -14596,17 +14593,30 @@
   </si>
   <si>
     <t>BCIO:050239</t>
+  </si>
+  <si>
+    <t>BCIO:036076</t>
+  </si>
+  <si>
+    <t>Impulsiveness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -14755,36 +14765,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -15036,8 +15047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5DA9F2-4651-473C-94DA-C36677DDFF52}">
   <dimension ref="A1:AL1517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H112" sqref="H112"/>
+    <sheetView tabSelected="1" topLeftCell="F988" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1003" sqref="G1003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16240,7 +16251,7 @@
         <v>171</v>
       </c>
       <c r="AC25" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.45">
@@ -18111,7 +18122,7 @@
         <v>306</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>4822</v>
+        <v>4821</v>
       </c>
       <c r="D65" t="s">
         <v>3000</v>
@@ -18135,7 +18146,7 @@
         <v>462</v>
       </c>
       <c r="AC65" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.45">
@@ -18343,7 +18354,7 @@
         <v>43</v>
       </c>
       <c r="AC70" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.45">
@@ -18745,7 +18756,7 @@
         <v>36</v>
       </c>
       <c r="AC79" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.45">
@@ -18818,7 +18829,7 @@
         <v>36</v>
       </c>
       <c r="AC81" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.45">
@@ -18985,7 +18996,7 @@
         <v>43</v>
       </c>
       <c r="AC85" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.45">
@@ -19208,7 +19219,7 @@
         <v>171</v>
       </c>
       <c r="AC90" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.45">
@@ -19293,7 +19304,7 @@
         <v>171</v>
       </c>
       <c r="AC92" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.45">
@@ -19384,7 +19395,7 @@
         <v>171</v>
       </c>
       <c r="AC94" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.45">
@@ -19475,7 +19486,7 @@
         <v>36</v>
       </c>
       <c r="AC96" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.45">
@@ -19636,7 +19647,7 @@
         <v>36</v>
       </c>
       <c r="AC100" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="101" spans="1:29" x14ac:dyDescent="0.45">
@@ -19753,7 +19764,7 @@
         <v>43</v>
       </c>
       <c r="AC103" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="104" spans="1:29" x14ac:dyDescent="0.45">
@@ -20099,7 +20110,7 @@
         <v>171</v>
       </c>
       <c r="AC111" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="112" spans="1:29" x14ac:dyDescent="0.45">
@@ -20134,7 +20145,7 @@
         <v>171</v>
       </c>
       <c r="AC112" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="113" spans="1:28" x14ac:dyDescent="0.45">
@@ -22627,10 +22638,10 @@
         <v>940</v>
       </c>
       <c r="C169" s="14" t="s">
+        <v>4827</v>
+      </c>
+      <c r="D169" s="19" t="s">
         <v>4828</v>
-      </c>
-      <c r="D169" s="19" t="s">
-        <v>4829</v>
       </c>
       <c r="E169" s="14" t="s">
         <v>65</v>
@@ -22664,7 +22675,7 @@
       <c r="Z169" s="14"/>
       <c r="AA169" s="14"/>
       <c r="AB169" s="14" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
       <c r="AC169" s="14"/>
     </row>
@@ -23373,7 +23384,7 @@
         <v>2496</v>
       </c>
       <c r="F186" s="11" t="s">
-        <v>4838</v>
+        <v>4837</v>
       </c>
       <c r="G186" t="s">
         <v>2497</v>
@@ -24777,7 +24788,7 @@
         <v>281</v>
       </c>
       <c r="F219" t="s">
-        <v>4837</v>
+        <v>4836</v>
       </c>
       <c r="G219" t="s">
         <v>1276</v>
@@ -27151,7 +27162,7 @@
         <v>43</v>
       </c>
       <c r="AC275" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="276" spans="1:29" x14ac:dyDescent="0.45">
@@ -27732,7 +27743,7 @@
         <v>171</v>
       </c>
       <c r="AC288" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="289" spans="1:27" x14ac:dyDescent="0.45">
@@ -31607,7 +31618,7 @@
         <v>36</v>
       </c>
       <c r="AC373" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="374" spans="1:29" x14ac:dyDescent="0.45">
@@ -31683,7 +31694,7 @@
         <v>43</v>
       </c>
       <c r="AC375" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="376" spans="1:29" x14ac:dyDescent="0.45">
@@ -31712,7 +31723,7 @@
         <v>43</v>
       </c>
       <c r="AC376" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="377" spans="1:29" x14ac:dyDescent="0.45">
@@ -31741,7 +31752,7 @@
         <v>43</v>
       </c>
       <c r="AC377" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="378" spans="1:29" x14ac:dyDescent="0.45">
@@ -31770,7 +31781,7 @@
         <v>43</v>
       </c>
       <c r="AC378" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="379" spans="1:29" x14ac:dyDescent="0.45">
@@ -31846,7 +31857,7 @@
         <v>43</v>
       </c>
       <c r="AC380" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="381" spans="1:29" x14ac:dyDescent="0.45">
@@ -31882,7 +31893,7 @@
         <v>43</v>
       </c>
       <c r="AC381" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="382" spans="1:29" x14ac:dyDescent="0.45">
@@ -31893,10 +31904,10 @@
         <v>521</v>
       </c>
       <c r="C382" t="s">
+        <v>4824</v>
+      </c>
+      <c r="D382" s="18" t="s">
         <v>4825</v>
-      </c>
-      <c r="D382" s="18" t="s">
-        <v>4826</v>
       </c>
       <c r="E382" s="18"/>
       <c r="F382" s="18" t="s">
@@ -31911,7 +31922,7 @@
       <c r="L382" s="18"/>
       <c r="M382" s="18"/>
       <c r="N382" s="18" t="s">
-        <v>4827</v>
+        <v>4826</v>
       </c>
       <c r="P382" s="18"/>
       <c r="Q382" s="18" t="s">
@@ -31944,7 +31955,7 @@
         <v>43</v>
       </c>
       <c r="AC383" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="384" spans="1:29" x14ac:dyDescent="0.45">
@@ -32020,7 +32031,7 @@
         <v>36</v>
       </c>
       <c r="AC385" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="386" spans="1:29" x14ac:dyDescent="0.45">
@@ -32096,7 +32107,7 @@
         <v>36</v>
       </c>
       <c r="AC387" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="388" spans="1:29" x14ac:dyDescent="0.45">
@@ -32131,7 +32142,7 @@
         <v>171</v>
       </c>
       <c r="AC388" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="389" spans="1:29" x14ac:dyDescent="0.45">
@@ -32166,7 +32177,7 @@
         <v>171</v>
       </c>
       <c r="AC389" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="390" spans="1:29" x14ac:dyDescent="0.45">
@@ -32207,7 +32218,7 @@
         <v>171</v>
       </c>
       <c r="AC390" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="391" spans="1:29" x14ac:dyDescent="0.45">
@@ -37689,7 +37700,7 @@
         <v>43</v>
       </c>
       <c r="AC512" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="513" spans="1:29" x14ac:dyDescent="0.45">
@@ -37988,7 +37999,7 @@
         <v>43</v>
       </c>
       <c r="AC519" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="520" spans="1:29" x14ac:dyDescent="0.45">
@@ -38017,7 +38028,7 @@
         <v>43</v>
       </c>
       <c r="AC520" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="521" spans="1:29" x14ac:dyDescent="0.45">
@@ -38269,7 +38280,7 @@
         <v>36</v>
       </c>
       <c r="AC526" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="527" spans="1:29" x14ac:dyDescent="0.45">
@@ -38298,7 +38309,7 @@
         <v>43</v>
       </c>
       <c r="AC527" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="528" spans="1:29" x14ac:dyDescent="0.45">
@@ -38327,7 +38338,7 @@
         <v>36</v>
       </c>
       <c r="AC528" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="529" spans="1:29" x14ac:dyDescent="0.45">
@@ -38356,7 +38367,7 @@
         <v>43</v>
       </c>
       <c r="AC529" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="530" spans="1:29" x14ac:dyDescent="0.45">
@@ -39504,7 +39515,7 @@
         <v>36</v>
       </c>
       <c r="AC554" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="555" spans="1:29" x14ac:dyDescent="0.45">
@@ -39941,7 +39952,7 @@
         <v>43</v>
       </c>
       <c r="AC564" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="565" spans="1:29" x14ac:dyDescent="0.45">
@@ -40827,7 +40838,7 @@
         <v>101</v>
       </c>
       <c r="AC584" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="585" spans="1:29" x14ac:dyDescent="0.45">
@@ -41481,7 +41492,7 @@
         <v>578</v>
       </c>
       <c r="D599" t="s">
-        <v>4820</v>
+        <v>4819</v>
       </c>
       <c r="F599" t="s">
         <v>579</v>
@@ -46210,7 +46221,7 @@
         <v>4203</v>
       </c>
       <c r="F700" t="s">
-        <v>4815</v>
+        <v>4814</v>
       </c>
       <c r="G700" t="s">
         <v>4204</v>
@@ -46982,7 +46993,7 @@
         <v>2762</v>
       </c>
       <c r="F717" t="s">
-        <v>4819</v>
+        <v>4818</v>
       </c>
       <c r="G717" t="s">
         <v>2763</v>
@@ -47202,7 +47213,7 @@
         <v>3375</v>
       </c>
       <c r="F722" t="s">
-        <v>4817</v>
+        <v>4816</v>
       </c>
       <c r="G722" t="s">
         <v>3376</v>
@@ -47246,10 +47257,10 @@
         <v>3690</v>
       </c>
       <c r="F723" t="s">
-        <v>4814</v>
+        <v>4813</v>
       </c>
       <c r="G723" t="s">
-        <v>4813</v>
+        <v>4812</v>
       </c>
       <c r="N723" t="s">
         <v>3691</v>
@@ -47340,7 +47351,7 @@
         <v>4064</v>
       </c>
       <c r="F725" t="s">
-        <v>4818</v>
+        <v>4817</v>
       </c>
       <c r="G725" t="s">
         <v>4065</v>
@@ -47428,7 +47439,7 @@
         <v>4233</v>
       </c>
       <c r="F727" t="s">
-        <v>4816</v>
+        <v>4815</v>
       </c>
       <c r="G727" t="s">
         <v>4234</v>
@@ -48052,7 +48063,7 @@
         <v>43</v>
       </c>
       <c r="AC739" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="740" spans="1:29" x14ac:dyDescent="0.45">
@@ -48125,7 +48136,7 @@
         <v>36</v>
       </c>
       <c r="AC741" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="742" spans="1:29" x14ac:dyDescent="0.45">
@@ -48811,13 +48822,13 @@
         <v>3953</v>
       </c>
       <c r="D757" t="s">
-        <v>4830</v>
+        <v>4829</v>
       </c>
       <c r="F757" s="11" t="s">
         <v>4041</v>
       </c>
       <c r="G757" s="12" t="s">
-        <v>4831</v>
+        <v>4830</v>
       </c>
       <c r="Q757" s="12" t="s">
         <v>43</v>
@@ -48946,7 +48957,7 @@
         <v>171</v>
       </c>
       <c r="AC760" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="761" spans="1:29" x14ac:dyDescent="0.45">
@@ -49160,7 +49171,7 @@
         <v>43</v>
       </c>
       <c r="AC765" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="766" spans="1:29" x14ac:dyDescent="0.45">
@@ -49377,7 +49388,7 @@
         <v>36</v>
       </c>
       <c r="AC770" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="771" spans="1:29" x14ac:dyDescent="0.45">
@@ -49453,7 +49464,7 @@
         <v>36</v>
       </c>
       <c r="AC772" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="773" spans="1:29" x14ac:dyDescent="0.45">
@@ -49614,7 +49625,7 @@
         <v>36</v>
       </c>
       <c r="AC776" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="777" spans="1:29" x14ac:dyDescent="0.45">
@@ -49734,7 +49745,7 @@
         <v>43</v>
       </c>
       <c r="AC779" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="780" spans="1:29" x14ac:dyDescent="0.45">
@@ -49760,7 +49771,7 @@
         <v>43</v>
       </c>
       <c r="AC780" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="781" spans="1:29" x14ac:dyDescent="0.45">
@@ -49836,7 +49847,7 @@
         <v>36</v>
       </c>
       <c r="AC782" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="783" spans="1:29" x14ac:dyDescent="0.45">
@@ -49865,7 +49876,7 @@
         <v>36</v>
       </c>
       <c r="AC783" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="784" spans="1:29" x14ac:dyDescent="0.45">
@@ -49941,7 +49952,7 @@
         <v>43</v>
       </c>
       <c r="AC785" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="786" spans="1:29" x14ac:dyDescent="0.45">
@@ -50521,7 +50532,7 @@
         <v>582</v>
       </c>
       <c r="D796" t="s">
-        <v>4820</v>
+        <v>4819</v>
       </c>
       <c r="F796" t="s">
         <v>579</v>
@@ -58387,7 +58398,7 @@
         <v>43</v>
       </c>
       <c r="AC967" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="968" spans="1:29" x14ac:dyDescent="0.45">
@@ -59165,10 +59176,10 @@
         <v>4724</v>
       </c>
       <c r="C984" t="s">
+        <v>4740</v>
+      </c>
+      <c r="D984" t="s">
         <v>4741</v>
-      </c>
-      <c r="D984" t="s">
-        <v>4742</v>
       </c>
       <c r="E984" t="s">
         <v>65</v>
@@ -59189,7 +59200,7 @@
         <v>462</v>
       </c>
       <c r="AC984" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="985" spans="1:29" x14ac:dyDescent="0.45">
@@ -59221,7 +59232,7 @@
         <v>462</v>
       </c>
       <c r="AC985" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="986" spans="1:29" x14ac:dyDescent="0.45">
@@ -59232,10 +59243,10 @@
         <v>4724</v>
       </c>
       <c r="C986" t="s">
+        <v>4743</v>
+      </c>
+      <c r="D986" t="s">
         <v>4744</v>
-      </c>
-      <c r="D986" t="s">
-        <v>4745</v>
       </c>
       <c r="E986" t="s">
         <v>65</v>
@@ -59256,7 +59267,7 @@
         <v>462</v>
       </c>
       <c r="AC986" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="987" spans="1:29" x14ac:dyDescent="0.45">
@@ -59270,19 +59281,19 @@
         <v>2427</v>
       </c>
       <c r="D987" t="s">
-        <v>4746</v>
+        <v>4745</v>
       </c>
       <c r="F987" t="s">
         <v>2426</v>
       </c>
       <c r="G987" t="s">
-        <v>4747</v>
+        <v>4746</v>
       </c>
       <c r="Q987" t="s">
         <v>43</v>
       </c>
       <c r="AC987" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="988" spans="1:29" x14ac:dyDescent="0.45">
@@ -59343,7 +59354,7 @@
         <v>77</v>
       </c>
       <c r="D989" t="s">
-        <v>4743</v>
+        <v>4742</v>
       </c>
       <c r="E989" t="s">
         <v>65</v>
@@ -59358,7 +59369,7 @@
         <v>43</v>
       </c>
       <c r="AC989" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="990" spans="1:29" x14ac:dyDescent="0.45">
@@ -59516,7 +59527,7 @@
         <v>65</v>
       </c>
       <c r="F993" t="s">
-        <v>4832</v>
+        <v>4831</v>
       </c>
       <c r="G993" t="s">
         <v>4729</v>
@@ -59525,7 +59536,7 @@
         <v>43</v>
       </c>
       <c r="AC993" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="994" spans="1:29" x14ac:dyDescent="0.45">
@@ -59598,7 +59609,7 @@
         <v>43</v>
       </c>
       <c r="AC995" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="996" spans="1:29" x14ac:dyDescent="0.45">
@@ -59888,16 +59899,16 @@
         <v>65</v>
       </c>
       <c r="F1002" t="s">
-        <v>4740</v>
-      </c>
-      <c r="G1002" t="s">
-        <v>4738</v>
+        <v>4838</v>
+      </c>
+      <c r="G1002" s="24" t="s">
+        <v>4839</v>
       </c>
       <c r="Q1002" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="AC1002" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1003" spans="1:29" x14ac:dyDescent="0.45">
@@ -59973,7 +59984,7 @@
         <v>43</v>
       </c>
       <c r="AC1004" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1005" spans="1:29" x14ac:dyDescent="0.45">
@@ -61791,7 +61802,7 @@
         <v>77</v>
       </c>
       <c r="D1043" t="s">
-        <v>4748</v>
+        <v>4747</v>
       </c>
       <c r="E1043" t="s">
         <v>65</v>
@@ -61806,7 +61817,7 @@
         <v>43</v>
       </c>
       <c r="AC1043" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1044" spans="1:29" x14ac:dyDescent="0.45">
@@ -61905,10 +61916,10 @@
         <v>463</v>
       </c>
       <c r="C1046" t="s">
+        <v>4748</v>
+      </c>
+      <c r="D1046" t="s">
         <v>4749</v>
-      </c>
-      <c r="D1046" t="s">
-        <v>4750</v>
       </c>
       <c r="E1046" t="s">
         <v>4696</v>
@@ -61923,7 +61934,7 @@
         <v>36</v>
       </c>
       <c r="AC1046" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1047" spans="1:29" x14ac:dyDescent="0.45">
@@ -62163,10 +62174,10 @@
         <v>463</v>
       </c>
       <c r="C1052" t="s">
+        <v>4753</v>
+      </c>
+      <c r="D1052" t="s">
         <v>4754</v>
-      </c>
-      <c r="D1052" t="s">
-        <v>4755</v>
       </c>
       <c r="E1052" t="s">
         <v>65</v>
@@ -62175,13 +62186,13 @@
         <v>3831</v>
       </c>
       <c r="G1052" t="s">
-        <v>4756</v>
+        <v>4755</v>
       </c>
       <c r="Q1052" t="s">
         <v>43</v>
       </c>
       <c r="AC1052" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1053" spans="1:29" x14ac:dyDescent="0.45">
@@ -62283,10 +62294,10 @@
         <v>463</v>
       </c>
       <c r="C1055" t="s">
+        <v>4750</v>
+      </c>
+      <c r="D1055" t="s">
         <v>4751</v>
-      </c>
-      <c r="D1055" t="s">
-        <v>4752</v>
       </c>
       <c r="E1055" t="s">
         <v>65</v>
@@ -62295,13 +62306,13 @@
         <v>3867</v>
       </c>
       <c r="G1055" t="s">
-        <v>4753</v>
+        <v>4752</v>
       </c>
       <c r="Q1055" t="s">
         <v>43</v>
       </c>
       <c r="AC1055" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1056" spans="1:29" x14ac:dyDescent="0.45">
@@ -67022,10 +67033,10 @@
         <v>539</v>
       </c>
       <c r="C1158" t="s">
+        <v>4756</v>
+      </c>
+      <c r="D1158" t="s">
         <v>4757</v>
-      </c>
-      <c r="D1158" t="s">
-        <v>4758</v>
       </c>
       <c r="F1158" t="s">
         <v>995</v>
@@ -67037,7 +67048,7 @@
         <v>43</v>
       </c>
       <c r="AC1158" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1159" spans="1:29" x14ac:dyDescent="0.45">
@@ -67398,16 +67409,16 @@
         <v>32</v>
       </c>
       <c r="F1166" s="11" t="s">
+        <v>4832</v>
+      </c>
+      <c r="G1166" s="23" t="s">
         <v>4833</v>
       </c>
-      <c r="G1166" s="23" t="s">
+      <c r="H1166" s="11" t="s">
         <v>4834</v>
       </c>
-      <c r="H1166" s="11" t="s">
+      <c r="I1166" s="23" t="s">
         <v>4835</v>
-      </c>
-      <c r="I1166" s="23" t="s">
-        <v>4836</v>
       </c>
       <c r="N1166" t="s">
         <v>1446</v>
@@ -67959,10 +67970,10 @@
         <v>399</v>
       </c>
       <c r="C1178" t="s">
+        <v>4775</v>
+      </c>
+      <c r="D1178" t="s">
         <v>4776</v>
-      </c>
-      <c r="D1178" t="s">
-        <v>4777</v>
       </c>
       <c r="E1178" t="s">
         <v>65</v>
@@ -67983,7 +67994,7 @@
         <v>462</v>
       </c>
       <c r="AC1178" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1179" spans="1:29" x14ac:dyDescent="0.45">
@@ -68135,10 +68146,10 @@
         <v>399</v>
       </c>
       <c r="C1182" t="s">
+        <v>4780</v>
+      </c>
+      <c r="D1182" t="s">
         <v>4781</v>
-      </c>
-      <c r="D1182" t="s">
-        <v>4782</v>
       </c>
       <c r="E1182" t="s">
         <v>65</v>
@@ -68153,7 +68164,7 @@
         <v>36</v>
       </c>
       <c r="AC1182" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1183" spans="1:29" x14ac:dyDescent="0.45">
@@ -68164,10 +68175,10 @@
         <v>399</v>
       </c>
       <c r="C1183" t="s">
+        <v>4758</v>
+      </c>
+      <c r="D1183" t="s">
         <v>4759</v>
-      </c>
-      <c r="D1183" t="s">
-        <v>4760</v>
       </c>
       <c r="E1183" t="s">
         <v>65</v>
@@ -68182,7 +68193,7 @@
         <v>43</v>
       </c>
       <c r="AC1183" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1184" spans="1:29" x14ac:dyDescent="0.45">
@@ -68334,25 +68345,25 @@
         <v>399</v>
       </c>
       <c r="C1187" t="s">
+        <v>4767</v>
+      </c>
+      <c r="D1187" t="s">
         <v>4768</v>
-      </c>
-      <c r="D1187" t="s">
-        <v>4769</v>
       </c>
       <c r="E1187" t="s">
         <v>65</v>
       </c>
       <c r="F1187" t="s">
+        <v>4769</v>
+      </c>
+      <c r="G1187" t="s">
         <v>4770</v>
-      </c>
-      <c r="G1187" t="s">
-        <v>4771</v>
       </c>
       <c r="Q1187" t="s">
         <v>36</v>
       </c>
       <c r="AC1187" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1188" spans="1:29" x14ac:dyDescent="0.45">
@@ -68460,7 +68471,7 @@
         <v>3887</v>
       </c>
       <c r="D1190" t="s">
-        <v>4766</v>
+        <v>4765</v>
       </c>
       <c r="E1190" t="s">
         <v>65</v>
@@ -68469,13 +68480,13 @@
         <v>3889</v>
       </c>
       <c r="G1190" t="s">
-        <v>4767</v>
+        <v>4766</v>
       </c>
       <c r="Q1190" t="s">
         <v>43</v>
       </c>
       <c r="AC1190" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1191" spans="1:29" x14ac:dyDescent="0.45">
@@ -68486,25 +68497,25 @@
         <v>399</v>
       </c>
       <c r="C1191" t="s">
+        <v>4761</v>
+      </c>
+      <c r="D1191" t="s">
         <v>4762</v>
-      </c>
-      <c r="D1191" t="s">
-        <v>4763</v>
       </c>
       <c r="E1191" t="s">
         <v>65</v>
       </c>
       <c r="F1191" t="s">
+        <v>4763</v>
+      </c>
+      <c r="G1191" t="s">
         <v>4764</v>
       </c>
-      <c r="G1191" t="s">
-        <v>4765</v>
-      </c>
       <c r="Q1191" t="s">
         <v>43</v>
       </c>
       <c r="AC1191" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1192" spans="1:29" x14ac:dyDescent="0.45">
@@ -68600,10 +68611,10 @@
         <v>399</v>
       </c>
       <c r="C1194" t="s">
+        <v>4771</v>
+      </c>
+      <c r="D1194" t="s">
         <v>4772</v>
-      </c>
-      <c r="D1194" t="s">
-        <v>4773</v>
       </c>
       <c r="E1194" t="s">
         <v>65</v>
@@ -68615,16 +68626,16 @@
         <v>1819</v>
       </c>
       <c r="H1194" t="s">
+        <v>4773</v>
+      </c>
+      <c r="I1194" t="s">
         <v>4774</v>
-      </c>
-      <c r="I1194" t="s">
-        <v>4775</v>
       </c>
       <c r="Q1194" t="s">
         <v>171</v>
       </c>
       <c r="AC1194" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1195" spans="1:29" x14ac:dyDescent="0.45">
@@ -68638,7 +68649,7 @@
         <v>2895</v>
       </c>
       <c r="D1195" t="s">
-        <v>4761</v>
+        <v>4760</v>
       </c>
       <c r="E1195" t="s">
         <v>65</v>
@@ -68659,7 +68670,7 @@
         <v>171</v>
       </c>
       <c r="AC1195" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1196" spans="1:29" x14ac:dyDescent="0.45">
@@ -68670,10 +68681,10 @@
         <v>399</v>
       </c>
       <c r="C1196" t="s">
+        <v>4777</v>
+      </c>
+      <c r="D1196" t="s">
         <v>4778</v>
-      </c>
-      <c r="D1196" t="s">
-        <v>4779</v>
       </c>
       <c r="E1196" t="s">
         <v>65</v>
@@ -68682,19 +68693,19 @@
         <v>1166</v>
       </c>
       <c r="G1196" t="s">
-        <v>4780</v>
+        <v>4779</v>
       </c>
       <c r="H1196" t="s">
         <v>3889</v>
       </c>
       <c r="I1196" t="s">
-        <v>4767</v>
+        <v>4766</v>
       </c>
       <c r="Q1196" t="s">
         <v>171</v>
       </c>
       <c r="AC1196" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1197" spans="1:29" x14ac:dyDescent="0.45">
@@ -79706,10 +79717,10 @@
         <v>193</v>
       </c>
       <c r="C1428" t="s">
-        <v>4823</v>
+        <v>4822</v>
       </c>
       <c r="D1428" t="s">
-        <v>4785</v>
+        <v>4784</v>
       </c>
       <c r="E1428" t="s">
         <v>65</v>
@@ -79724,7 +79735,7 @@
         <v>43</v>
       </c>
       <c r="AC1428" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1429" spans="1:29" x14ac:dyDescent="0.45">
@@ -79735,10 +79746,10 @@
         <v>193</v>
       </c>
       <c r="C1429" t="s">
+        <v>4782</v>
+      </c>
+      <c r="D1429" t="s">
         <v>4783</v>
-      </c>
-      <c r="D1429" t="s">
-        <v>4784</v>
       </c>
       <c r="F1429" t="s">
         <v>995</v>
@@ -79750,7 +79761,7 @@
         <v>36</v>
       </c>
       <c r="AC1429" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1430" spans="1:29" x14ac:dyDescent="0.45">
@@ -79761,10 +79772,10 @@
         <v>193</v>
       </c>
       <c r="C1430" s="9" t="s">
-        <v>4824</v>
+        <v>4823</v>
       </c>
       <c r="D1430" t="s">
-        <v>4788</v>
+        <v>4787</v>
       </c>
       <c r="E1430" t="s">
         <v>65</v>
@@ -79779,7 +79790,7 @@
         <v>43</v>
       </c>
       <c r="AC1430" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1431" spans="1:29" x14ac:dyDescent="0.45">
@@ -79931,10 +79942,10 @@
         <v>193</v>
       </c>
       <c r="C1434" t="s">
+        <v>4785</v>
+      </c>
+      <c r="D1434" t="s">
         <v>4786</v>
-      </c>
-      <c r="D1434" t="s">
-        <v>4787</v>
       </c>
       <c r="E1434" t="s">
         <v>65</v>
@@ -79949,7 +79960,7 @@
         <v>43</v>
       </c>
       <c r="AC1434" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1435" spans="1:29" x14ac:dyDescent="0.45">
@@ -80145,7 +80156,7 @@
         <v>193</v>
       </c>
       <c r="C1439" s="7" t="s">
-        <v>4821</v>
+        <v>4820</v>
       </c>
       <c r="D1439" t="s">
         <v>1055</v>
@@ -80198,10 +80209,10 @@
         <v>193</v>
       </c>
       <c r="C1440" t="s">
+        <v>4792</v>
+      </c>
+      <c r="D1440" t="s">
         <v>4793</v>
-      </c>
-      <c r="D1440" t="s">
-        <v>4794</v>
       </c>
       <c r="E1440" t="s">
         <v>65</v>
@@ -80213,16 +80224,16 @@
         <v>1054</v>
       </c>
       <c r="H1440" t="s">
+        <v>4790</v>
+      </c>
+      <c r="I1440" t="s">
         <v>4791</v>
-      </c>
-      <c r="I1440" t="s">
-        <v>4792</v>
       </c>
       <c r="Q1440" t="s">
         <v>171</v>
       </c>
       <c r="AC1440" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1441" spans="1:29" x14ac:dyDescent="0.45">
@@ -80233,10 +80244,10 @@
         <v>193</v>
       </c>
       <c r="C1441" t="s">
+        <v>4788</v>
+      </c>
+      <c r="D1441" t="s">
         <v>4789</v>
-      </c>
-      <c r="D1441" t="s">
-        <v>4790</v>
       </c>
       <c r="E1441" t="s">
         <v>65</v>
@@ -80248,16 +80259,16 @@
         <v>1737</v>
       </c>
       <c r="H1441" t="s">
+        <v>4790</v>
+      </c>
+      <c r="I1441" t="s">
         <v>4791</v>
-      </c>
-      <c r="I1441" t="s">
-        <v>4792</v>
       </c>
       <c r="Q1441" t="s">
         <v>171</v>
       </c>
       <c r="AC1441" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1442" spans="1:29" x14ac:dyDescent="0.45">
@@ -82311,19 +82322,19 @@
         <v>82</v>
       </c>
       <c r="B1484" t="s">
-        <v>4795</v>
+        <v>4794</v>
       </c>
       <c r="C1484" t="s">
+        <v>4803</v>
+      </c>
+      <c r="D1484" t="s">
         <v>4804</v>
-      </c>
-      <c r="D1484" t="s">
-        <v>4805</v>
       </c>
       <c r="Q1484" t="s">
         <v>101</v>
       </c>
       <c r="AC1484" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1485" spans="1:29" x14ac:dyDescent="0.45">
@@ -82378,19 +82389,19 @@
         <v>82</v>
       </c>
       <c r="B1486" t="s">
-        <v>4795</v>
+        <v>4794</v>
       </c>
       <c r="C1486" t="s">
+        <v>4797</v>
+      </c>
+      <c r="D1486" t="s">
         <v>4798</v>
-      </c>
-      <c r="D1486" t="s">
-        <v>4799</v>
       </c>
       <c r="Q1486" t="s">
         <v>101</v>
       </c>
       <c r="AC1486" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1487" spans="1:29" x14ac:dyDescent="0.45">
@@ -82586,19 +82597,19 @@
         <v>82</v>
       </c>
       <c r="B1491" t="s">
-        <v>4795</v>
+        <v>4794</v>
       </c>
       <c r="C1491" t="s">
+        <v>4801</v>
+      </c>
+      <c r="D1491" t="s">
         <v>4802</v>
-      </c>
-      <c r="D1491" t="s">
-        <v>4803</v>
       </c>
       <c r="Q1491" t="s">
         <v>101</v>
       </c>
       <c r="AC1491" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1492" spans="1:29" x14ac:dyDescent="0.45">
@@ -82606,19 +82617,19 @@
         <v>82</v>
       </c>
       <c r="B1492" t="s">
-        <v>4795</v>
+        <v>4794</v>
       </c>
       <c r="C1492" t="s">
+        <v>4799</v>
+      </c>
+      <c r="D1492" t="s">
         <v>4800</v>
-      </c>
-      <c r="D1492" t="s">
-        <v>4801</v>
       </c>
       <c r="Q1492" t="s">
         <v>101</v>
       </c>
       <c r="AC1492" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1493" spans="1:29" x14ac:dyDescent="0.45">
@@ -82905,19 +82916,19 @@
         <v>82</v>
       </c>
       <c r="B1499" t="s">
+        <v>4794</v>
+      </c>
+      <c r="C1499" t="s">
         <v>4795</v>
       </c>
-      <c r="C1499" t="s">
+      <c r="D1499" t="s">
         <v>4796</v>
-      </c>
-      <c r="D1499" t="s">
-        <v>4797</v>
       </c>
       <c r="Q1499" t="s">
         <v>101</v>
       </c>
       <c r="AC1499" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1500" spans="1:29" x14ac:dyDescent="0.45">
@@ -83019,13 +83030,13 @@
         <v>82</v>
       </c>
       <c r="B1502" t="s">
-        <v>4795</v>
+        <v>4794</v>
       </c>
       <c r="C1502" t="s">
+        <v>4805</v>
+      </c>
+      <c r="D1502" t="s">
         <v>4806</v>
-      </c>
-      <c r="D1502" t="s">
-        <v>4807</v>
       </c>
       <c r="E1502" t="s">
         <v>65</v>
@@ -83037,16 +83048,16 @@
         <v>3087</v>
       </c>
       <c r="H1502" t="s">
+        <v>4807</v>
+      </c>
+      <c r="I1502" t="s">
         <v>4808</v>
-      </c>
-      <c r="I1502" t="s">
-        <v>4809</v>
       </c>
       <c r="Q1502" t="s">
         <v>171</v>
       </c>
       <c r="AC1502" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1503" spans="1:29" x14ac:dyDescent="0.45">
@@ -83166,7 +83177,7 @@
         <v>4613</v>
       </c>
       <c r="D1505" t="s">
-        <v>4810</v>
+        <v>4809</v>
       </c>
       <c r="E1505" t="s">
         <v>65</v>
@@ -83181,7 +83192,7 @@
         <v>43</v>
       </c>
       <c r="AC1505" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1506" spans="1:29" x14ac:dyDescent="0.45">
@@ -83286,7 +83297,7 @@
         <v>4615</v>
       </c>
       <c r="D1508" t="s">
-        <v>4811</v>
+        <v>4810</v>
       </c>
       <c r="E1508" t="s">
         <v>65</v>
@@ -83301,7 +83312,7 @@
         <v>43</v>
       </c>
       <c r="AC1508" t="s">
-        <v>4812</v>
+        <v>4811</v>
       </c>
     </row>
     <row r="1509" spans="1:29" x14ac:dyDescent="0.45">
@@ -83743,29 +83754,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8b526686-74c6-4282-acd2-1df788241888">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="21a5e57e-4e60-422b-854b-a13449c3b6f7" xsi:nil="true"/>
-    <Notes xmlns="8b526686-74c6-4282-acd2-1df788241888" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F51F80E9A93DB844AF2178C388C5A380" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2bc01d953c63a8b00c496244ab16aded">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8b526686-74c6-4282-acd2-1df788241888" xmlns:ns3="21a5e57e-4e60-422b-854b-a13449c3b6f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01bfba5c6ea6d6282822bcba6e0fda49" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F51F80E9A93DB844AF2178C388C5A380" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5b9ddb339475d5ae1032a1a9aad75d5">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8b526686-74c6-4282-acd2-1df788241888" xmlns:ns3="21a5e57e-4e60-422b-854b-a13449c3b6f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="32357b74feaf063910b38d4f222a5807" ns2:_="" ns3:_="">
     <xsd:import namespace="8b526686-74c6-4282-acd2-1df788241888"/>
     <xsd:import namespace="21a5e57e-4e60-422b-854b-a13449c3b6f7"/>
     <xsd:element name="properties">
@@ -83786,6 +83776,7 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:Notes" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -83855,6 +83846,11 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="21" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -83972,21 +83968,29 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8b526686-74c6-4282-acd2-1df788241888">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="21a5e57e-4e60-422b-854b-a13449c3b6f7" xsi:nil="true"/>
+    <Notes xmlns="8b526686-74c6-4282-acd2-1df788241888" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEB898B8-86B9-4CB5-911E-3D0C2D4B0B23}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="21a5e57e-4e60-422b-854b-a13449c3b6f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8b526686-74c6-4282-acd2-1df788241888"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C60E9E64-7FEE-4660-8752-0F7F070BE576}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -83998,20 +84002,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAD7B01D-AD2E-4C65-AE22-150B1C2B7E64}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEB898B8-86B9-4CB5-911E-3D0C2D4B0B23}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="21a5e57e-4e60-422b-854b-a13449c3b6f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8b526686-74c6-4282-acd2-1df788241888"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8b526686-74c6-4282-acd2-1df788241888"/>
-    <ds:schemaRef ds:uri="21a5e57e-4e60-422b-854b-a13449c3b6f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>